<commit_message>
Realização do DML e DQL do exercício 1.3
</commit_message>
<xml_diff>
--- a/exercicios/1.3-exercicio-pclinics/MODELAGEM/01_exercicio-pclinics-modelagem_fisico.xlsx
+++ b/exercicios/1.3-exercicio-pclinics/MODELAGEM/01_exercicio-pclinics-modelagem_fisico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\senai_sprint1_bd\exercicios\1.3-exercicio-pclinics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\senai_sprint1_bd\exercicios\1.3-exercicio-pclinics\MODELAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180D840-6B4E-4D91-9A74-1646C76B13CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F98E8E8-6542-4660-A165-88C2B05F103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{54DF69EB-125F-4421-B953-676CCA66AA30}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Clinica</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Felipe</t>
   </si>
   <si>
-    <t>Shi-tzu</t>
-  </si>
-  <si>
     <t>Salsicha</t>
   </si>
   <si>
@@ -142,6 +139,21 @@
   </si>
   <si>
     <t>valor</t>
+  </si>
+  <si>
+    <t>Shih-tzu</t>
+  </si>
+  <si>
+    <t>Sphynx</t>
+  </si>
+  <si>
+    <t>Persa</t>
+  </si>
+  <si>
+    <t>Mangalarga</t>
+  </si>
+  <si>
+    <t>Cavalo</t>
   </si>
 </sst>
 </file>
@@ -175,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,57 +210,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -256,13 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D49443-432F-44EE-8635-736330B41A9F}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,31 +568,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="1"/>
@@ -641,49 +607,49 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="S2" s="1"/>
@@ -700,49 +666,49 @@
       <c r="AD2" s="1"/>
     </row>
     <row r="3" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <v>1</v>
-      </c>
-      <c r="L3" s="8">
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
         <v>44312</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="8">
         <v>75</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="6">
-        <v>1</v>
-      </c>
-      <c r="P3" s="5" t="s">
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="6">
-        <v>1</v>
-      </c>
-      <c r="R3" s="6">
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
+      <c r="R3" s="5">
         <v>3</v>
       </c>
       <c r="S3" s="1"/>
@@ -759,50 +725,50 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="6">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="6">
-        <v>2</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5">
         <v>3</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>4</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>44314</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="8">
         <v>75</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="6">
-        <v>2</v>
-      </c>
-      <c r="P4" s="5" t="s">
+      <c r="O4" s="5">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="6">
-        <v>1</v>
-      </c>
-      <c r="R4" s="6">
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
         <v>3</v>
       </c>
       <c r="S4" s="1"/>
@@ -823,42 +789,42 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>3</v>
       </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6">
-        <v>2</v>
-      </c>
-      <c r="L5" s="8">
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7">
         <v>44321</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>90</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>3</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="6">
-        <v>2</v>
-      </c>
-      <c r="R5" s="6">
+      <c r="Q5" s="5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="5">
         <v>1</v>
       </c>
       <c r="S5" s="1"/>
@@ -883,32 +849,32 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>4</v>
       </c>
-      <c r="J6" s="6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="J6" s="5">
+        <v>2</v>
+      </c>
+      <c r="K6" s="5">
         <v>3</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>44337</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="8">
         <v>105</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>4</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="6">
+      <c r="Q6" s="5">
+        <v>2</v>
+      </c>
+      <c r="R6" s="5">
         <v>2</v>
       </c>
       <c r="S6" s="1"/>
@@ -989,21 +955,21 @@
       <c r="AD8" s="1"/>
     </row>
     <row r="9" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="I9" s="4" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="I9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1026,27 +992,27 @@
       <c r="AD9" s="1"/>
     </row>
     <row r="10" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="1"/>
@@ -1071,29 +1037,29 @@
       <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="5">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>35</v>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1117,29 +1083,29 @@
       <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="5">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6">
-        <v>2</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="6">
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="5">
         <v>1</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="6">
-        <v>2</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>36</v>
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1163,26 +1129,30 @@
       <c r="AD12" s="1"/>
     </row>
     <row r="13" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6">
-        <v>2</v>
+      <c r="F13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="1"/>
+      <c r="I13" s="5">
+        <v>3</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1209,9 +1179,15 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="E14" s="5">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
@@ -1241,9 +1217,15 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1273,9 +1255,15 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="E16" s="5">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="5">
+        <v>3</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>

</xml_diff>